<commit_message>
add pdf in data directory
</commit_message>
<xml_diff>
--- a/Data/Sample.xlsx
+++ b/Data/Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dean\Project\Project\private\TesPer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\GitTesPer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB0C270-A627-4CBD-B5E1-10329401C09C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AA25DB-8672-4009-9CBB-AD78E46080B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8655" xr2:uid="{973FA397-4C36-499A-9426-6601ED227441}"/>
+    <workbookView xWindow="28845" yWindow="3060" windowWidth="21570" windowHeight="15345" xr2:uid="{973FA397-4C36-499A-9426-6601ED227441}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -99,9 +99,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -121,9 +124,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -161,7 +164,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -267,7 +270,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -409,7 +412,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -417,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B7DEE1-DB0C-4E0C-BA61-19AE00470976}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.375" customWidth="1"/>
+    <col min="1" max="3" width="87.875" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -445,6 +448,484 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>